<commit_message>
Correct part for 10nF capacitors
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -73,10 +73,10 @@
     <t xml:space="preserve">10n</t>
   </si>
   <si>
-    <t xml:space="preserve">C0603C103K4RAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80-C0603C103K4RAC</t>
+    <t xml:space="preserve">C0603C103K2RECTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0603C103K2REC</t>
   </si>
   <si>
     <t xml:space="preserve">C7</t>

</xml_diff>

<commit_message>
Change Case code for 47u caps
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="232">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -154,31 +154,34 @@
     <t xml:space="preserve">81-GRM188R61C475KAJD</t>
   </si>
   <si>
+    <t xml:space="preserve">C26;C27;C31;C34;C36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitors_Tantalum_SMD:CP_EIA-6032-28_Kemet-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAJC476K016SNJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">581-TAJC476K016SNJ</t>
+  </si>
+  <si>
     <t xml:space="preserve">C1;C5</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitors_Tantalum_SMD:CP_Tantalum_Case-A_EIA-3216-18_Reflow</t>
   </si>
   <si>
-    <t xml:space="preserve">AVX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THJA106K006AJN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">581-THJA106K006AJN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C26;C27;C31;C34;C36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47u</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F931A476KAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">647-F931A476KAA</t>
+    <t xml:space="preserve">F931C106KAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">647-F931C106KAA</t>
   </si>
   <si>
     <t xml:space="preserve">J7</t>
@@ -1066,62 +1069,62 @@
         <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -1129,13 +1132,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -1143,117 +1146,117 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1</v>
@@ -1262,30 +1265,30 @@
         <v>41</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>742863160</v>
@@ -1294,278 +1297,278 @@
         <v>13</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5</v>
@@ -1573,19 +1576,19 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>61300411121</v>
@@ -1594,24 +1597,24 @@
         <v>13</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>61300411121</v>
@@ -1620,24 +1623,24 @@
         <v>13</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>61300711121</v>
@@ -1646,553 +1649,553 @@
         <v>13</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G46" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>330</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>5</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C51" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="D51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>212</v>
-      </c>
       <c r="G51" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C52" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F52" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="D52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>216</v>
-      </c>
       <c r="G52" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BOM and README for rev0.2
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -127,7 +127,7 @@
     <t xml:space="preserve">80-C0603C393K4R</t>
   </si>
   <si>
-    <t xml:space="preserve">C14;C15</t>
+    <t xml:space="preserve">C14;C15;C6</t>
   </si>
   <si>
     <t xml:space="preserve">470p</t>
@@ -424,10 +424,10 @@
     <t xml:space="preserve">J5</t>
   </si>
   <si>
-    <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_1x07_Pitch2.54mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">710-61300711121</t>
+    <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_1x08_Pitch2.54mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710-61300811121</t>
   </si>
   <si>
     <t xml:space="preserve">J4</t>
@@ -613,7 +613,7 @@
     <t xml:space="preserve">667-ERJ-3EKF3002V</t>
   </si>
   <si>
-    <t xml:space="preserve">R13;R14</t>
+    <t xml:space="preserve">R13;R14;R35</t>
   </si>
   <si>
     <t xml:space="preserve">ERJ-U03F3300V</t>
@@ -622,7 +622,7 @@
     <t xml:space="preserve">667-ERJ-U03F3300V</t>
   </si>
   <si>
-    <t xml:space="preserve">R16;R12;R18</t>
+    <t xml:space="preserve">R16;R12;R18;R34</t>
   </si>
   <si>
     <t xml:space="preserve">47k</t>
@@ -685,7 +685,7 @@
     <t xml:space="preserve">512-2N7002</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1</t>
+    <t xml:space="preserve">Q1;Q3</t>
   </si>
   <si>
     <t xml:space="preserve">IRLML2060</t>
@@ -813,8 +813,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1023,7 +1023,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>11</v>
@@ -1643,7 +1643,7 @@
         <v>90</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>61300711121</v>
+        <v>61300811121</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>13</v>
@@ -2001,7 +2001,7 @@
         <v>169</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>170</v>
@@ -2027,7 +2027,7 @@
         <v>169</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>170</v>
@@ -2157,7 +2157,7 @@
         <v>218</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>223</v>

</xml_diff>

<commit_message>
Update PCB layout to rev0.3
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="234">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -394,6 +394,12 @@
     <t xml:space="preserve">604-APT1608SECK</t>
   </si>
   <si>
+    <t xml:space="preserve">D11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FM</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP3;TP4;TP2;TP5;TP1</t>
   </si>
   <si>
@@ -436,16 +442,16 @@
     <t xml:space="preserve">Panel LEDs</t>
   </si>
   <si>
-    <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_2x10_Pitch2.00mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3M Electronic Solutions Division</t>
-  </si>
-  <si>
-    <t xml:space="preserve">951210-8622-AR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">517-951210-8622-AR</t>
+    <t xml:space="preserve">Connector_PinHeader_2.00mm:PinHeader_2x11_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samtec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTMM-111-09-L-D-380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200-MTMM11109LD380</t>
   </si>
   <si>
     <t xml:space="preserve">J2</t>
@@ -565,7 +571,7 @@
     <t xml:space="preserve">667-ERJ-3EKF1001V</t>
   </si>
   <si>
-    <t xml:space="preserve">R1;R2;R4;R5;R6;R7;R8;R9;R11;R33</t>
+    <t xml:space="preserve">R1;R2;R4;R5;R6;R7;R8;R9;R11;R33;R36</t>
   </si>
   <si>
     <t xml:space="preserve">1k5</t>
@@ -796,12 +802,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -811,23 +817,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="103.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1568,47 +1573,47 @@
         <v>125</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="C31" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>129</v>
-      </c>
       <c r="D31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>61300411121</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
@@ -1623,7 +1628,7 @@
         <v>13</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,10 +1636,10 @@
         <v>133</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
@@ -1643,559 +1648,585 @@
         <v>90</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>61300811121</v>
+        <v>61300411121</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="D34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>61300811121</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="G35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="G36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="G37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="G38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="G39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C40" s="0" t="s">
+      <c r="G40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="G41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="G42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F43" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="G43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="G44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="G45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="G46" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F47" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>330</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F47" s="0" t="s">
+      <c r="G47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>330</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="G48" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="0" t="s">
         <v>201</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F49" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="G49" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F50" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="G50" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="0" t="s">
         <v>209</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="F51" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="G51" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="0" t="s">
         <v>213</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="D51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="D52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="0" t="s">
         <v>217</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="F53" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="F54" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="G54" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="C54" s="0" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="D54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E54" s="0" t="s">
+      <c r="B55" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="F54" s="0" t="s">
+      <c r="C55" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="G54" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H54" s="0" t="s">
+      <c r="D55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>231</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>